<commit_message>
Pre-processing failed due to unselected columns, so removed or modified them
</commit_message>
<xml_diff>
--- a/CLR/CLR_standard_input_mac_low.xlsx
+++ b/CLR/CLR_standard_input_mac_low.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="638">
   <si>
     <t>text</t>
   </si>
@@ -3117,10 +3117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3137,11 +3137,10 @@
     <col min="11" max="11" width="53.140625" style="3" customWidth="1"/>
     <col min="12" max="13" width="39.140625" style="3" customWidth="1"/>
     <col min="14" max="14" width="42.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="44.5703125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="84.28515625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>337</v>
       </c>
@@ -3161,7 +3160,7 @@
         <v>95</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>516</v>
+        <v>525</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>486</v>
@@ -3176,22 +3175,19 @@
         <v>620</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>518</v>
+        <v>342</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>519</v>
+        <v>490</v>
       </c>
       <c r="N1" s="16" t="s">
         <v>459</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>521</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
@@ -3229,7 +3225,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$C$2:$C$15</xm:f>
@@ -3268,15 +3264,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$H$1:$H$7</xm:f>
+            <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
           <xm:sqref>O1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>P1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>

</xml_diff>